<commit_message>
generateDriveCycle work, no 2nd axis
</commit_message>
<xml_diff>
--- a/2_Drive_Cycle_Generation/time_speed_elevation_distance_theta_data.xlsx
+++ b/2_Drive_Cycle_Generation/time_speed_elevation_distance_theta_data.xlsx
@@ -56,10 +56,10 @@
   <dimension ref="A1:E2881"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="true"/>
-    <col min="2" max="2" width="12.7109375" customWidth="true"/>
+    <col min="1" max="1" width="11.7109375" customWidth="true"/>
+    <col min="2" max="2" width="13.7109375" customWidth="true"/>
     <col min="3" max="3" width="9.7109375" customWidth="true"/>
-    <col min="4" max="4" width="10.7109375" customWidth="true"/>
+    <col min="4" max="4" width="6.7109375" customWidth="true"/>
     <col min="5" max="5" width="16.42578125" customWidth="true"/>
   </cols>
   <sheetData>
@@ -82,10 +82,10 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>0.7009011243386245</v>
+        <v>1.1315926484976626</v>
       </c>
       <c r="B2" s="0">
-        <v>1.282565130260521</v>
+        <v>1.1155866900175131</v>
       </c>
       <c r="C2" s="0">
         <v>0.035737999999999999</v>
@@ -99,10 +99,10 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>1.401802248677249</v>
+        <v>2.2631852969953252</v>
       </c>
       <c r="B3" s="0">
-        <v>1.7955911823647295</v>
+        <v>1.5691768826619967</v>
       </c>
       <c r="C3" s="0">
         <v>0.10496999999999999</v>
@@ -116,10 +116,10 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>2.1027033730158733</v>
+        <v>3.3947779454929878</v>
       </c>
       <c r="B4" s="0">
-        <v>2.1963927855711423</v>
+        <v>1.9246935201401052</v>
       </c>
       <c r="C4" s="0">
         <v>0.10772</v>
@@ -133,10 +133,10 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>2.803604497354498</v>
+        <v>4.5263705939906504</v>
       </c>
       <c r="B5" s="0">
-        <v>2.5330661322645289</v>
+        <v>2.2189141856392296</v>
       </c>
       <c r="C5" s="0">
         <v>0.14341000000000001</v>
@@ -150,10 +150,10 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>3.5045056216931223</v>
+        <v>5.6579632424883126</v>
       </c>
       <c r="B6" s="0">
-        <v>2.8216432865731464</v>
+        <v>2.4763572679509633</v>
       </c>
       <c r="C6" s="0">
         <v>0.18539</v>
@@ -167,10 +167,10 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>4.2054067460317466</v>
+        <v>6.7895558909859757</v>
       </c>
       <c r="B7" s="0">
-        <v>3.1102204408817635</v>
+        <v>2.7215411558669</v>
       </c>
       <c r="C7" s="0">
         <v>0.24281</v>
@@ -184,10 +184,10 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>4.9063078703703713</v>
+        <v>7.921148539483637</v>
       </c>
       <c r="B8" s="0">
-        <v>3.3507014028056115</v>
+        <v>2.9299474605954465</v>
       </c>
       <c r="C8" s="0">
         <v>0.26534000000000002</v>
@@ -201,10 +201,10 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>5.607208994708996</v>
+        <v>9.0527411879813009</v>
       </c>
       <c r="B9" s="0">
-        <v>3.5751503006012024</v>
+        <v>3.1383537653239935</v>
       </c>
       <c r="C9" s="0">
         <v>0.30620999999999998</v>
@@ -218,10 +218,10 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>6.3081101190476199</v>
+        <v>10.184333836478963</v>
       </c>
       <c r="B10" s="0">
-        <v>3.7995991983967934</v>
+        <v>3.3222416812609459</v>
       </c>
       <c r="C10" s="0">
         <v>0.34432000000000001</v>
@@ -235,10 +235,10 @@
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>7.0090112433862446</v>
+        <v>11.315926484976625</v>
       </c>
       <c r="B11" s="0">
-        <v>4.0080160320641287</v>
+        <v>3.5061295971978987</v>
       </c>
       <c r="C11" s="0">
         <v>0.36324000000000001</v>
@@ -252,10 +252,10 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>7.7099123677248702</v>
+        <v>12.447519133474287</v>
       </c>
       <c r="B12" s="0">
-        <v>4.2004008016032071</v>
+        <v>3.6777583187390546</v>
       </c>
       <c r="C12" s="0">
         <v>0.40839999999999999</v>
@@ -269,10 +269,10 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>8.4108134920634932</v>
+        <v>13.579111781971951</v>
       </c>
       <c r="B13" s="0">
-        <v>4.376753507014028</v>
+        <v>3.8371278458844134</v>
       </c>
       <c r="C13" s="0">
         <v>0.44874000000000003</v>
@@ -286,10 +286,10 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>9.1117146164021179</v>
+        <v>14.710704430469614</v>
       </c>
       <c r="B14" s="0">
-        <v>4.5531062124248498</v>
+        <v>3.996497373029773</v>
       </c>
       <c r="C14" s="0">
         <v>0.50744999999999996</v>
@@ -303,10 +303,10 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>9.8126157407407426</v>
+        <v>15.842297078967274</v>
       </c>
       <c r="B15" s="0">
-        <v>4.7294589178356707</v>
+        <v>4.1436077057793339</v>
       </c>
       <c r="C15" s="0">
         <v>0.52866000000000002</v>
@@ -320,10 +320,10 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>10.513516865079367</v>
+        <v>16.973889727464936</v>
       </c>
       <c r="B16" s="0">
-        <v>4.9058116232464934</v>
+        <v>4.2907180385288965</v>
       </c>
       <c r="C16" s="0">
         <v>0.54874000000000001</v>
@@ -337,10 +337,10 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>11.214417989417992</v>
+        <v>18.105482375962602</v>
       </c>
       <c r="B17" s="0">
-        <v>5.0661322645290578</v>
+        <v>4.4255691768826626</v>
       </c>
       <c r="C17" s="0">
         <v>0.58008000000000004</v>
@@ -354,10 +354,10 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>11.915319113756615</v>
+        <v>19.237075024460264</v>
       </c>
       <c r="B18" s="0">
-        <v>5.2104208416833675</v>
+        <v>4.5604203152364278</v>
       </c>
       <c r="C18" s="0">
         <v>0.60309000000000001</v>
@@ -371,10 +371,10 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>12.61622023809524</v>
+        <v>20.368667672957926</v>
       </c>
       <c r="B19" s="0">
-        <v>5.3707414829659319</v>
+        <v>4.6952714535901929</v>
       </c>
       <c r="C19" s="0">
         <v>0.64756000000000002</v>
@@ -388,10 +388,10 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>13.317121362433866</v>
+        <v>21.500260321455588</v>
       </c>
       <c r="B20" s="0">
-        <v>5.5150300601202398</v>
+        <v>4.8301225919439572</v>
       </c>
       <c r="C20" s="0">
         <v>0.69913000000000003</v>
@@ -405,10 +405,10 @@
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>14.018022486772489</v>
+        <v>22.63185296995325</v>
       </c>
       <c r="B21" s="0">
-        <v>5.6593186372745494</v>
+        <v>4.9527145359019267</v>
       </c>
       <c r="C21" s="0">
         <v>0.73436999999999997</v>
@@ -422,10 +422,10 @@
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>14.718923611111114</v>
+        <v>23.763445618450916</v>
       </c>
       <c r="B22" s="0">
-        <v>5.8036072144288573</v>
+        <v>5.0753064798598952</v>
       </c>
       <c r="C22" s="0">
         <v>0.77664999999999995</v>
@@ -439,10 +439,10 @@
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>15.41982473544974</v>
+        <v>24.895038266948575</v>
       </c>
       <c r="B23" s="0">
-        <v>5.9318637274549095</v>
+        <v>5.1978984238178638</v>
       </c>
       <c r="C23" s="0">
         <v>0.80147000000000002</v>
@@ -456,10 +456,10 @@
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>16.120725859788365</v>
+        <v>26.026630915446237</v>
       </c>
       <c r="B24" s="0">
-        <v>6.0761523046092183</v>
+        <v>5.3082311733800358</v>
       </c>
       <c r="C24" s="0">
         <v>0.83079999999999998</v>
@@ -473,10 +473,10 @@
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>16.821626984126986</v>
+        <v>27.158223563943903</v>
       </c>
       <c r="B25" s="0">
-        <v>6.2044088176352705</v>
+        <v>5.4185639229422069</v>
       </c>
       <c r="C25" s="0">
         <v>0.85946999999999996</v>
@@ -490,10 +490,10 @@
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>17.522528108465611</v>
+        <v>28.289816212441565</v>
       </c>
       <c r="B26" s="0">
-        <v>6.3326653306613228</v>
+        <v>5.5411558669001764</v>
       </c>
       <c r="C26" s="0">
         <v>0.91471000000000002</v>
@@ -507,10 +507,10 @@
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>18.223429232804236</v>
+        <v>29.421408860939227</v>
       </c>
       <c r="B27" s="0">
-        <v>6.4448897795591193</v>
+        <v>5.63922942206655</v>
       </c>
       <c r="C27" s="0">
         <v>0.98699999999999999</v>
@@ -524,10 +524,10 @@
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>18.92433035714286</v>
+        <v>30.553001509436893</v>
       </c>
       <c r="B28" s="0">
-        <v>6.5731462925851707</v>
+        <v>5.749562171628722</v>
       </c>
       <c r="C28" s="0">
         <v>1.0446</v>
@@ -541,10 +541,10 @@
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>19.625231481481485</v>
+        <v>31.684594157934548</v>
       </c>
       <c r="B29" s="0">
-        <v>6.7014028056112229</v>
+        <v>5.8598949211908931</v>
       </c>
       <c r="C29" s="0">
         <v>1.1265000000000001</v>
@@ -558,10 +558,10 @@
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>20.32613260582011</v>
+        <v>32.816186806432214</v>
       </c>
       <c r="B30" s="0">
-        <v>6.8136272545090186</v>
+        <v>5.9579684763572685</v>
       </c>
       <c r="C30" s="0">
         <v>1.1976</v>
@@ -575,10 +575,10 @@
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>21.027033730158735</v>
+        <v>33.947779454929872</v>
       </c>
       <c r="B31" s="0">
-        <v>6.9258517034068134</v>
+        <v>6.0683012259194395</v>
       </c>
       <c r="C31" s="0">
         <v>1.2977000000000001</v>
@@ -592,10 +592,10 @@
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>21.727934854497359</v>
+        <v>35.079372103427538</v>
       </c>
       <c r="B32" s="0">
-        <v>7.0380761523046091</v>
+        <v>6.1663747810858149</v>
       </c>
       <c r="C32" s="0">
         <v>1.4260999999999999</v>
@@ -609,10 +609,10 @@
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>22.428835978835984</v>
+        <v>36.210964751925204</v>
       </c>
       <c r="B33" s="0">
-        <v>7.1503006012024048</v>
+        <v>6.2644483362521886</v>
       </c>
       <c r="C33" s="0">
         <v>1.5533999999999999</v>
@@ -626,10 +626,10 @@
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>23.129737103174609</v>
+        <v>37.342557400422862</v>
       </c>
       <c r="B34" s="0">
-        <v>7.2625250501002006</v>
+        <v>6.3625218914185648</v>
       </c>
       <c r="C34" s="0">
         <v>1.7002999999999999</v>
@@ -643,10 +643,10 @@
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>23.83063822751323</v>
+        <v>38.474150048920528</v>
       </c>
       <c r="B35" s="0">
-        <v>7.3747494989979963</v>
+        <v>6.4605954465849393</v>
       </c>
       <c r="C35" s="0">
         <v>1.8176000000000001</v>
@@ -660,10 +660,10 @@
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>24.531539351851855</v>
+        <v>39.605742697418194</v>
       </c>
       <c r="B36" s="0">
-        <v>7.4869739478957911</v>
+        <v>6.5464098073555173</v>
       </c>
       <c r="C36" s="0">
         <v>1.8384</v>
@@ -677,10 +677,10 @@
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>25.232440476190479</v>
+        <v>40.737335345915852</v>
       </c>
       <c r="B37" s="0">
-        <v>7.5991983967935868</v>
+        <v>6.6444833625218918</v>
       </c>
       <c r="C37" s="0">
         <v>1.8898999999999999</v>
@@ -694,10 +694,10 @@
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>25.933341600529108</v>
+        <v>41.868927994413511</v>
       </c>
       <c r="B38" s="0">
-        <v>7.6953907815631259</v>
+        <v>6.7302977232924697</v>
       </c>
       <c r="C38" s="0">
         <v>1.9590000000000001</v>
@@ -711,10 +711,10 @@
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>26.634242724867732</v>
+        <v>43.000520642911177</v>
       </c>
       <c r="B39" s="0">
-        <v>7.7915831663326651</v>
+        <v>6.8283712784588442</v>
       </c>
       <c r="C39" s="0">
         <v>2.0057</v>
@@ -728,10 +728,10 @@
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>27.335143849206357</v>
+        <v>44.132113291408842</v>
       </c>
       <c r="B40" s="0">
-        <v>7.9038076152304608</v>
+        <v>6.9141856392294221</v>
       </c>
       <c r="C40" s="0">
         <v>2.0065</v>
@@ -745,10 +745,10 @@
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>28.036044973544978</v>
+        <v>45.263705939906501</v>
       </c>
       <c r="B41" s="0">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C41" s="0">
         <v>2.1076000000000001</v>
@@ -762,10 +762,10 @@
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>28.736946097883603</v>
+        <v>46.395298588404167</v>
       </c>
       <c r="B42" s="0">
-        <v>8</v>
+        <v>7.1590909090909092</v>
       </c>
       <c r="C42" s="0">
         <v>2.2170999999999998</v>
@@ -779,10 +779,10 @@
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>29.437847222222228</v>
+        <v>47.526891236901832</v>
       </c>
       <c r="B43" s="0">
-        <v>8</v>
+        <v>7.3181818181818183</v>
       </c>
       <c r="C43" s="0">
         <v>2.3643000000000001</v>
@@ -796,10 +796,10 @@
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>30.138748346560853</v>
+        <v>48.658483885399491</v>
       </c>
       <c r="B44" s="0">
-        <v>8</v>
+        <v>7.4545454545454541</v>
       </c>
       <c r="C44" s="0">
         <v>2.5291000000000001</v>
@@ -813,10 +813,10 @@
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>30.839649470899481</v>
+        <v>49.79007653389715</v>
       </c>
       <c r="B45" s="0">
-        <v>8</v>
+        <v>7.6136363636363633</v>
       </c>
       <c r="C45" s="0">
         <v>2.6873</v>
@@ -830,10 +830,10 @@
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>31.540550595238106</v>
+        <v>50.921669182394815</v>
       </c>
       <c r="B46" s="0">
-        <v>8</v>
+        <v>7.75</v>
       </c>
       <c r="C46" s="0">
         <v>2.8418999999999999</v>
@@ -847,10 +847,10 @@
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>32.24145171957673</v>
+        <v>52.053261830892474</v>
       </c>
       <c r="B47" s="0">
-        <v>8</v>
+        <v>7.7983870967741939</v>
       </c>
       <c r="C47" s="0">
         <v>3.0316999999999998</v>
@@ -864,10 +864,10 @@
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>32.942352843915351</v>
+        <v>53.18485447939014</v>
       </c>
       <c r="B48" s="0">
-        <v>8</v>
+        <v>7.854838709677419</v>
       </c>
       <c r="C48" s="0">
         <v>3.1583000000000001</v>
@@ -881,10 +881,10 @@
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>33.643253968253973</v>
+        <v>54.316447127887805</v>
       </c>
       <c r="B49" s="0">
-        <v>8</v>
+        <v>7.903225806451613</v>
       </c>
       <c r="C49" s="0">
         <v>3.2784</v>
@@ -898,10 +898,10 @@
     </row>
     <row r="50">
       <c r="A50" s="0">
-        <v>34.344155092592601</v>
+        <v>55.448039776385464</v>
       </c>
       <c r="B50" s="0">
-        <v>8</v>
+        <v>7.9516129032258061</v>
       </c>
       <c r="C50" s="0">
         <v>3.4201999999999999</v>
@@ -915,7 +915,7 @@
     </row>
     <row r="51">
       <c r="A51" s="0">
-        <v>35.045056216931222</v>
+        <v>56.57963242488313</v>
       </c>
       <c r="B51" s="0">
         <v>8</v>
@@ -932,10 +932,10 @@
     </row>
     <row r="52">
       <c r="A52" s="0">
-        <v>35.74595734126985</v>
+        <v>57.711225073380788</v>
       </c>
       <c r="B52" s="0">
-        <v>8</v>
+        <v>7.5263157894736841</v>
       </c>
       <c r="C52" s="0">
         <v>3.6082999999999998</v>
@@ -949,10 +949,10 @@
     </row>
     <row r="53">
       <c r="A53" s="0">
-        <v>36.446858465608472</v>
+        <v>58.842817721878454</v>
       </c>
       <c r="B53" s="0">
-        <v>8</v>
+        <v>6.9736842105263159</v>
       </c>
       <c r="C53" s="0">
         <v>3.6875</v>
@@ -966,10 +966,10 @@
     </row>
     <row r="54">
       <c r="A54" s="0">
-        <v>37.1477595899471</v>
+        <v>59.974410370376113</v>
       </c>
       <c r="B54" s="0">
-        <v>8</v>
+        <v>6.3421052631578947</v>
       </c>
       <c r="C54" s="0">
         <v>3.8081999999999998</v>
@@ -983,10 +983,10 @@
     </row>
     <row r="55">
       <c r="A55" s="0">
-        <v>37.848660714285721</v>
+        <v>61.106003018873785</v>
       </c>
       <c r="B55" s="0">
-        <v>8</v>
+        <v>5.7105263157894743</v>
       </c>
       <c r="C55" s="0">
         <v>3.9548999999999999</v>
@@ -1000,10 +1000,10 @@
     </row>
     <row r="56">
       <c r="A56" s="0">
-        <v>38.549561838624349</v>
+        <v>62.237595667371437</v>
       </c>
       <c r="B56" s="0">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C56" s="0">
         <v>4.0884</v>
@@ -1017,10 +1017,10 @@
     </row>
     <row r="57">
       <c r="A57" s="0">
-        <v>39.25046296296297</v>
+        <v>63.369188315869096</v>
       </c>
       <c r="B57" s="0">
-        <v>8</v>
+        <v>4.67741935483871</v>
       </c>
       <c r="C57" s="0">
         <v>4.2275999999999998</v>
@@ -1034,10 +1034,10 @@
     </row>
     <row r="58">
       <c r="A58" s="0">
-        <v>39.951364087301599</v>
+        <v>64.500780964366768</v>
       </c>
       <c r="B58" s="0">
-        <v>8</v>
+        <v>4.32258064516129</v>
       </c>
       <c r="C58" s="0">
         <v>4.3234000000000004</v>
@@ -1051,10 +1051,10 @@
     </row>
     <row r="59">
       <c r="A59" s="0">
-        <v>40.65226521164022</v>
+        <v>65.632373612864427</v>
       </c>
       <c r="B59" s="0">
-        <v>7.669724770642202</v>
+        <v>3.903225806451613</v>
       </c>
       <c r="C59" s="0">
         <v>4.4291</v>
@@ -1068,10 +1068,10 @@
     </row>
     <row r="60">
       <c r="A60" s="0">
-        <v>41.353166335978841</v>
+        <v>66.7639662613621</v>
       </c>
       <c r="B60" s="0">
-        <v>7.2844036697247709</v>
+        <v>3.4838709677419351</v>
       </c>
       <c r="C60" s="0">
         <v>4.4828999999999999</v>
@@ -1085,10 +1085,10 @@
     </row>
     <row r="61">
       <c r="A61" s="0">
-        <v>42.054067460317469</v>
+        <v>67.895558909859744</v>
       </c>
       <c r="B61" s="0">
-        <v>6.8990825688073398</v>
+        <v>3</v>
       </c>
       <c r="C61" s="0">
         <v>4.5449000000000002</v>
@@ -1102,10 +1102,10 @@
     </row>
     <row r="62">
       <c r="A62" s="0">
-        <v>42.754968584656098</v>
+        <v>69.027151558357417</v>
       </c>
       <c r="B62" s="0">
-        <v>6.5137614678899087</v>
+        <v>2</v>
       </c>
       <c r="C62" s="0">
         <v>4.6100000000000003</v>
@@ -1119,10 +1119,10 @@
     </row>
     <row r="63">
       <c r="A63" s="0">
-        <v>43.455869708994719</v>
+        <v>70.158744206855076</v>
       </c>
       <c r="B63" s="0">
-        <v>6.0733944954128445</v>
+        <v>2</v>
       </c>
       <c r="C63" s="0">
         <v>4.6479999999999997</v>
@@ -1136,10 +1136,10 @@
     </row>
     <row r="64">
       <c r="A64" s="0">
-        <v>44.15677083333334</v>
+        <v>71.290336855352749</v>
       </c>
       <c r="B64" s="0">
-        <v>5.5779816513761471</v>
+        <v>2</v>
       </c>
       <c r="C64" s="0">
         <v>4.6727999999999996</v>
@@ -1153,10 +1153,10 @@
     </row>
     <row r="65">
       <c r="A65" s="0">
-        <v>44.857671957671968</v>
+        <v>72.421929503850407</v>
       </c>
       <c r="B65" s="0">
-        <v>5.0825688073394497</v>
+        <v>2</v>
       </c>
       <c r="C65" s="0">
         <v>4.6917</v>
@@ -1170,10 +1170,10 @@
     </row>
     <row r="66">
       <c r="A66" s="0">
-        <v>45.558573082010589</v>
+        <v>73.553522152348066</v>
       </c>
       <c r="B66" s="0">
-        <v>4.5321100917431192</v>
+        <v>2</v>
       </c>
       <c r="C66" s="0">
         <v>4.7362000000000002</v>
@@ -1187,10 +1187,10 @@
     </row>
     <row r="67">
       <c r="A67" s="0">
-        <v>46.259474206349218</v>
+        <v>74.685114800845724</v>
       </c>
       <c r="B67" s="0">
-        <v>3.8715596330275233</v>
+        <v>2.1726618705035969</v>
       </c>
       <c r="C67" s="0">
         <v>4.7312000000000003</v>
@@ -1204,10 +1204,10 @@
     </row>
     <row r="68">
       <c r="A68" s="0">
-        <v>46.960375330687839</v>
+        <v>75.816707449343383</v>
       </c>
       <c r="B68" s="0">
-        <v>3.0458715596330279</v>
+        <v>2.3309352517985609</v>
       </c>
       <c r="C68" s="0">
         <v>4.7492000000000001</v>
@@ -1221,10 +1221,10 @@
     </row>
     <row r="69">
       <c r="A69" s="0">
-        <v>47.66127645502646</v>
+        <v>76.948300097841056</v>
       </c>
       <c r="B69" s="0">
-        <v>2</v>
+        <v>2.4820143884892087</v>
       </c>
       <c r="C69" s="0">
         <v>4.7603</v>
@@ -1238,10 +1238,10 @@
     </row>
     <row r="70">
       <c r="A70" s="0">
-        <v>48.362177579365088</v>
+        <v>78.079892746338714</v>
       </c>
       <c r="B70" s="0">
-        <v>3.225806451612903</v>
+        <v>2.6187050359712227</v>
       </c>
       <c r="C70" s="0">
         <v>4.7026000000000003</v>
@@ -1255,10 +1255,10 @@
     </row>
     <row r="71">
       <c r="A71" s="0">
-        <v>49.063078703703709</v>
+        <v>79.211485394836387</v>
       </c>
       <c r="B71" s="0">
-        <v>4.129032258064516</v>
+        <v>2.7553956834532372</v>
       </c>
       <c r="C71" s="0">
         <v>4.6627999999999998</v>
@@ -1272,10 +1272,10 @@
     </row>
     <row r="72">
       <c r="A72" s="0">
-        <v>49.763979828042338</v>
+        <v>80.343078043334046</v>
       </c>
       <c r="B72" s="0">
-        <v>4.838709677419355</v>
+        <v>2.8776978417266186</v>
       </c>
       <c r="C72" s="0">
         <v>4.5688000000000004</v>
@@ -1289,10 +1289,10 @@
     </row>
     <row r="73">
       <c r="A73" s="0">
-        <v>50.464880952380959</v>
+        <v>81.474670691831705</v>
       </c>
       <c r="B73" s="0">
-        <v>5.4193548387096779</v>
+        <v>3</v>
       </c>
       <c r="C73" s="0">
         <v>4.3907999999999996</v>
@@ -1306,10 +1306,10 @@
     </row>
     <row r="74">
       <c r="A74" s="0">
-        <v>51.165782076719594</v>
+        <v>82.606263340329363</v>
       </c>
       <c r="B74" s="0">
-        <v>6</v>
+        <v>2.5135135135135136</v>
       </c>
       <c r="C74" s="0">
         <v>4.1746999999999996</v>
@@ -1323,10 +1323,10 @@
     </row>
     <row r="75">
       <c r="A75" s="0">
-        <v>51.866683201058216</v>
+        <v>83.737855988827022</v>
       </c>
       <c r="B75" s="0">
-        <v>5.5344827586206895</v>
+        <v>1.9189189189189189</v>
       </c>
       <c r="C75" s="0">
         <v>3.9563000000000001</v>
@@ -1340,10 +1340,10 @@
     </row>
     <row r="76">
       <c r="A76" s="0">
-        <v>52.567584325396837</v>
+        <v>84.869448637324695</v>
       </c>
       <c r="B76" s="0">
-        <v>5.068965517241379</v>
+        <v>1</v>
       </c>
       <c r="C76" s="0">
         <v>3.7561</v>
@@ -1357,10 +1357,10 @@
     </row>
     <row r="77">
       <c r="A77" s="0">
-        <v>53.268485449735465</v>
+        <v>86.001041285822353</v>
       </c>
       <c r="B77" s="0">
-        <v>4.5517241379310347</v>
+        <v>0.81605351170568563</v>
       </c>
       <c r="C77" s="0">
         <v>3.5983999999999998</v>
@@ -1374,10 +1374,10 @@
     </row>
     <row r="78">
       <c r="A78" s="0">
-        <v>53.969386574074086</v>
+        <v>87.132633934320026</v>
       </c>
       <c r="B78" s="0">
-        <v>3.9310344827586206</v>
+        <v>0.5752508361204014</v>
       </c>
       <c r="C78" s="0">
         <v>3.5352999999999999</v>
@@ -1391,10 +1391,10 @@
     </row>
     <row r="79">
       <c r="A79" s="0">
-        <v>54.670287698412714</v>
+        <v>88.264226582817685</v>
       </c>
       <c r="B79" s="0">
-        <v>3.2068965517241375</v>
+        <v>0.036789297658862873</v>
       </c>
       <c r="C79" s="0">
         <v>3.4615</v>
@@ -1408,10 +1408,10 @@
     </row>
     <row r="80">
       <c r="A80" s="0">
-        <v>55.371188822751336</v>
+        <v>89.395819231315343</v>
       </c>
       <c r="B80" s="0">
-        <v>2.2758620689655173</v>
+        <v>0.58193979933110362</v>
       </c>
       <c r="C80" s="0">
         <v>3.4504999999999999</v>
@@ -1425,10 +1425,10 @@
     </row>
     <row r="81">
       <c r="A81" s="0">
-        <v>56.072089947089957</v>
+        <v>90.527411879813002</v>
       </c>
       <c r="B81" s="0">
-        <v>0.17670682730923695</v>
+        <v>0.8193979933110368</v>
       </c>
       <c r="C81" s="0">
         <v>3.4657</v>
@@ -1442,10 +1442,10 @@
     </row>
     <row r="82">
       <c r="A82" s="0">
-        <v>56.772991071428585</v>
+        <v>91.65900452831066</v>
       </c>
       <c r="B82" s="0">
-        <v>1.2690763052208835</v>
+        <v>1</v>
       </c>
       <c r="C82" s="0">
         <v>3.5032000000000001</v>
@@ -1459,10 +1459,10 @@
     </row>
     <row r="83">
       <c r="A83" s="0">
-        <v>57.473892195767206</v>
+        <v>92.790597176808333</v>
       </c>
       <c r="B83" s="0">
-        <v>1.7991967871485943</v>
+        <v>1.5369127516778525</v>
       </c>
       <c r="C83" s="0">
         <v>3.4510999999999998</v>
@@ -1476,10 +1476,10 @@
     </row>
     <row r="84">
       <c r="A84" s="0">
-        <v>58.174793320105827</v>
+        <v>93.922189825305992</v>
       </c>
       <c r="B84" s="0">
-        <v>2.1847389558232932</v>
+        <v>1.912751677852349</v>
       </c>
       <c r="C84" s="0">
         <v>3.3952</v>
@@ -1493,10 +1493,10 @@
     </row>
     <row r="85">
       <c r="A85" s="0">
-        <v>58.875694444444456</v>
+        <v>95.053782473803665</v>
       </c>
       <c r="B85" s="0">
-        <v>2.5381526104417671</v>
+        <v>2.2348993288590604</v>
       </c>
       <c r="C85" s="0">
         <v>3.3656000000000001</v>
@@ -1510,10 +1510,10 @@
     </row>
     <row r="86">
       <c r="A86" s="0">
-        <v>59.576595568783077</v>
+        <v>96.185375122301309</v>
       </c>
       <c r="B86" s="0">
-        <v>2.8273092369477912</v>
+        <v>2.5167785234899327</v>
       </c>
       <c r="C86" s="0">
         <v>3.2732000000000001</v>
@@ -1527,10 +1527,10 @@
     </row>
     <row r="87">
       <c r="A87" s="0">
-        <v>60.277496693121705</v>
+        <v>97.316967770798982</v>
       </c>
       <c r="B87" s="0">
-        <v>3.1004016064257032</v>
+        <v>2.7718120805369129</v>
       </c>
       <c r="C87" s="0">
         <v>3.1978</v>
@@ -1544,10 +1544,10 @@
     </row>
     <row r="88">
       <c r="A88" s="0">
-        <v>60.978397817460326</v>
+        <v>98.448560419296641</v>
       </c>
       <c r="B88" s="0">
-        <v>3.3413654618473898</v>
+        <v>3</v>
       </c>
       <c r="C88" s="0">
         <v>3.1787000000000001</v>
@@ -1561,10 +1561,10 @@
     </row>
     <row r="89">
       <c r="A89" s="0">
-        <v>61.679298941798962</v>
+        <v>99.580153067794299</v>
       </c>
       <c r="B89" s="0">
-        <v>3.5823293172690764</v>
+        <v>3.1882352941176473</v>
       </c>
       <c r="C89" s="0">
         <v>3.3637000000000001</v>
@@ -1578,10 +1578,10 @@
     </row>
     <row r="90">
       <c r="A90" s="0">
-        <v>62.380200066137583</v>
+        <v>100.71174571629197</v>
       </c>
       <c r="B90" s="0">
-        <v>3.7911646586345382</v>
+        <v>3.3647058823529412</v>
       </c>
       <c r="C90" s="0">
         <v>3.6768000000000001</v>
@@ -1595,10 +1595,10 @@
     </row>
     <row r="91">
       <c r="A91" s="0">
-        <v>63.081101190476211</v>
+        <v>101.84333836478963</v>
       </c>
       <c r="B91" s="0">
-        <v>4</v>
+        <v>3.5411764705882351</v>
       </c>
       <c r="C91" s="0">
         <v>4.0236999999999998</v>
@@ -1612,10 +1612,10 @@
     </row>
     <row r="92">
       <c r="A92" s="0">
-        <v>63.782002314814832</v>
+        <v>102.97493101328729</v>
       </c>
       <c r="B92" s="0">
-        <v>3.7373737373737375</v>
+        <v>3.7058823529411766</v>
       </c>
       <c r="C92" s="0">
         <v>4.3273000000000001</v>
@@ -1629,10 +1629,10 @@
     </row>
     <row r="93">
       <c r="A93" s="0">
-        <v>64.482903439153461</v>
+        <v>104.10652366178495</v>
       </c>
       <c r="B93" s="0">
-        <v>3.4545454545454546</v>
+        <v>3.8470588235294119</v>
       </c>
       <c r="C93" s="0">
         <v>4.5621</v>
@@ -1646,10 +1646,10 @@
     </row>
     <row r="94">
       <c r="A94" s="0">
-        <v>65.183804563492075</v>
+        <v>105.23811631028262</v>
       </c>
       <c r="B94" s="0">
-        <v>3.1717171717171717</v>
+        <v>4</v>
       </c>
       <c r="C94" s="0">
         <v>4.7455999999999996</v>
@@ -1663,10 +1663,10 @@
     </row>
     <row r="95">
       <c r="A95" s="0">
-        <v>65.884705687830703</v>
+        <v>106.36970895878028</v>
       </c>
       <c r="B95" s="0">
-        <v>2.8282828282828278</v>
+        <v>4.3636363636363633</v>
       </c>
       <c r="C95" s="0">
         <v>4.8380999999999998</v>
@@ -1680,10 +1680,10 @@
     </row>
     <row r="96">
       <c r="A96" s="0">
-        <v>66.585606812169331</v>
+        <v>107.50130160727795</v>
       </c>
       <c r="B96" s="0">
-        <v>2.4444444444444446</v>
+        <v>4.6969696969696972</v>
       </c>
       <c r="C96" s="0">
         <v>4.8198999999999996</v>
@@ -1697,10 +1697,10 @@
     </row>
     <row r="97">
       <c r="A97" s="0">
-        <v>67.286507936507945</v>
+        <v>108.63289425577561</v>
       </c>
       <c r="B97" s="0">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C97" s="0">
         <v>4.8295000000000003</v>
@@ -1714,10 +1714,10 @@
     </row>
     <row r="98">
       <c r="A98" s="0">
-        <v>67.987409060846574</v>
+        <v>109.76448690427327</v>
       </c>
       <c r="B98" s="0">
-        <v>3.1111111111111112</v>
+        <v>5.330578512396694</v>
       </c>
       <c r="C98" s="0">
         <v>4.8346</v>
@@ -1731,10 +1731,10 @@
     </row>
     <row r="99">
       <c r="A99" s="0">
-        <v>68.688310185185202</v>
+        <v>110.89607955277093</v>
       </c>
       <c r="B99" s="0">
-        <v>3.988304093567252</v>
+        <v>5.6280991735537187</v>
       </c>
       <c r="C99" s="0">
         <v>4.8056999999999999</v>
@@ -1748,10 +1748,10 @@
     </row>
     <row r="100">
       <c r="A100" s="0">
-        <v>69.389211309523816</v>
+        <v>112.02767220126859</v>
       </c>
       <c r="B100" s="0">
-        <v>4.6315789473684212</v>
+        <v>5.9256198347107443</v>
       </c>
       <c r="C100" s="0">
         <v>4.7222999999999997</v>
@@ -1765,10 +1765,10 @@
     </row>
     <row r="101">
       <c r="A101" s="0">
-        <v>70.090112433862444</v>
+        <v>113.15926484976626</v>
       </c>
       <c r="B101" s="0">
-        <v>5.2163742690058479</v>
+        <v>6.1900826446280988</v>
       </c>
       <c r="C101" s="0">
         <v>4.6332000000000004</v>
@@ -1782,10 +1782,10 @@
     </row>
     <row r="102">
       <c r="A102" s="0">
-        <v>70.791013558201072</v>
+        <v>114.29085749826393</v>
       </c>
       <c r="B102" s="0">
-        <v>5.742690058479532</v>
+        <v>6.4545454545454541</v>
       </c>
       <c r="C102" s="0">
         <v>4.5412999999999997</v>
@@ -1799,10 +1799,10 @@
     </row>
     <row r="103">
       <c r="A103" s="0">
-        <v>71.491914682539701</v>
+        <v>115.42245014676158</v>
       </c>
       <c r="B103" s="0">
-        <v>6.269005847953216</v>
+        <v>6.6859504132231402</v>
       </c>
       <c r="C103" s="0">
         <v>4.4621000000000004</v>
@@ -1816,10 +1816,10 @@
     </row>
     <row r="104">
       <c r="A104" s="0">
-        <v>72.192815806878315</v>
+        <v>116.55404279525925</v>
       </c>
       <c r="B104" s="0">
-        <v>6.6783625730994149</v>
+        <v>6.9504132231404956</v>
       </c>
       <c r="C104" s="0">
         <v>4.3113999999999999</v>
@@ -1833,10 +1833,10 @@
     </row>
     <row r="105">
       <c r="A105" s="0">
-        <v>72.893716931216943</v>
+        <v>117.68563544375691</v>
       </c>
       <c r="B105" s="0">
-        <v>7.1461988304093564</v>
+        <v>7.1818181818181817</v>
       </c>
       <c r="C105" s="0">
         <v>4.2161999999999997</v>
@@ -1850,10 +1850,10 @@
     </row>
     <row r="106">
       <c r="A106" s="0">
-        <v>73.594618055555571</v>
+        <v>118.81722809225455</v>
       </c>
       <c r="B106" s="0">
-        <v>7.4970760233918128</v>
+        <v>7.3801652892561984</v>
       </c>
       <c r="C106" s="0">
         <v>4.1340000000000003</v>
@@ -1867,10 +1867,10 @@
     </row>
     <row r="107">
       <c r="A107" s="0">
-        <v>74.2955191798942</v>
+        <v>119.94882074075223</v>
       </c>
       <c r="B107" s="0">
-        <v>7.9064327485380117</v>
+        <v>7.6115702479338836</v>
       </c>
       <c r="C107" s="0">
         <v>4.0624000000000002</v>
@@ -1884,10 +1884,10 @@
     </row>
     <row r="108">
       <c r="A108" s="0">
-        <v>74.996420304232828</v>
+        <v>121.0804133892499</v>
       </c>
       <c r="B108" s="0">
-        <v>8.257309941520468</v>
+        <v>7.8099173553719003</v>
       </c>
       <c r="C108" s="0">
         <v>3.9908999999999999</v>
@@ -1901,10 +1901,10 @@
     </row>
     <row r="109">
       <c r="A109" s="0">
-        <v>75.697321428571442</v>
+        <v>122.21200603774757</v>
       </c>
       <c r="B109" s="0">
-        <v>8.6081871345029235</v>
+        <v>8.0413223140495873</v>
       </c>
       <c r="C109" s="0">
         <v>3.9346000000000001</v>
@@ -1918,10 +1918,10 @@
     </row>
     <row r="110">
       <c r="A110" s="0">
-        <v>76.39822255291007</v>
+        <v>123.34359868624522</v>
       </c>
       <c r="B110" s="0">
-        <v>8.9590643274853807</v>
+        <v>8.2396694214876032</v>
       </c>
       <c r="C110" s="0">
         <v>3.8595000000000002</v>
@@ -1935,10 +1935,10 @@
     </row>
     <row r="111">
       <c r="A111" s="0">
-        <v>77.099123677248699</v>
+        <v>124.47519133474287</v>
       </c>
       <c r="B111" s="0">
-        <v>9.2514619883040936</v>
+        <v>8.438016528925619</v>
       </c>
       <c r="C111" s="0">
         <v>3.8050999999999999</v>
@@ -1952,10 +1952,10 @@
     </row>
     <row r="112">
       <c r="A112" s="0">
-        <v>77.800024801587313</v>
+        <v>125.60678398324055</v>
       </c>
       <c r="B112" s="0">
-        <v>9.5438596491228083</v>
+        <v>8.6363636363636367</v>
       </c>
       <c r="C112" s="0">
         <v>3.7334999999999998</v>
@@ -1969,10 +1969,10 @@
     </row>
     <row r="113">
       <c r="A113" s="0">
-        <v>78.500925925925941</v>
+        <v>126.73837663173819</v>
       </c>
       <c r="B113" s="0">
-        <v>9.8947368421052637</v>
+        <v>8.8347107438016526</v>
       </c>
       <c r="C113" s="0">
         <v>3.6562999999999999</v>
@@ -1986,10 +1986,10 @@
     </row>
     <row r="114">
       <c r="A114" s="0">
-        <v>79.201827050264569</v>
+        <v>127.86996928023586</v>
       </c>
       <c r="B114" s="0">
-        <v>10.187134502923977</v>
+        <v>9</v>
       </c>
       <c r="C114" s="0">
         <v>3.5990000000000002</v>
@@ -2003,10 +2003,10 @@
     </row>
     <row r="115">
       <c r="A115" s="0">
-        <v>79.902728174603197</v>
+        <v>129.00156192873354</v>
       </c>
       <c r="B115" s="0">
-        <v>10.421052631578947</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="C115" s="0">
         <v>3.5571999999999999</v>
@@ -2020,10 +2020,10 @@
     </row>
     <row r="116">
       <c r="A116" s="0">
-        <v>80.603629298941811</v>
+        <v>130.13315457723121</v>
       </c>
       <c r="B116" s="0">
-        <v>10.713450292397662</v>
+        <v>9.3666666666666671</v>
       </c>
       <c r="C116" s="0">
         <v>3.5131000000000001</v>
@@ -2037,10 +2037,10 @@
     </row>
     <row r="117">
       <c r="A117" s="0">
-        <v>81.30453042328044</v>
+        <v>131.26474722572885</v>
       </c>
       <c r="B117" s="0">
-        <v>11.005847953216374</v>
+        <v>9.5333333333333332</v>
       </c>
       <c r="C117" s="0">
         <v>3.4390999999999998</v>
@@ -2054,10 +2054,10 @@
     </row>
     <row r="118">
       <c r="A118" s="0">
-        <v>82.005431547619068</v>
+        <v>132.39633987422653</v>
       </c>
       <c r="B118" s="0">
-        <v>11.239766081871345</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="C118" s="0">
         <v>3.3567</v>
@@ -2071,10 +2071,10 @@
     </row>
     <row r="119">
       <c r="A119" s="0">
-        <v>82.706332671957682</v>
+        <v>133.5279325227242</v>
       </c>
       <c r="B119" s="0">
-        <v>11.532163742690059</v>
+        <v>9.8666666666666671</v>
       </c>
       <c r="C119" s="0">
         <v>3.2757000000000001</v>
@@ -2088,10 +2088,10 @@
     </row>
     <row r="120">
       <c r="A120" s="0">
-        <v>83.40723379629631</v>
+        <v>134.65952517122184</v>
       </c>
       <c r="B120" s="0">
-        <v>11.766081871345028</v>
+        <v>10.033333333333333</v>
       </c>
       <c r="C120" s="0">
         <v>3.2378999999999998</v>
@@ -2105,10 +2105,10 @@
     </row>
     <row r="121">
       <c r="A121" s="0">
-        <v>84.108134920634939</v>
+        <v>135.79111781971949</v>
       </c>
       <c r="B121" s="0">
-        <v>12</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="C121" s="0">
         <v>3.1674000000000002</v>
@@ -2122,10 +2122,10 @@
     </row>
     <row r="122">
       <c r="A122" s="0">
-        <v>84.809036044973567</v>
+        <v>136.92271046821716</v>
       </c>
       <c r="B122" s="0">
-        <v>12</v>
+        <v>10.366666666666667</v>
       </c>
       <c r="C122" s="0">
         <v>3.0848</v>
@@ -2139,10 +2139,10 @@
     </row>
     <row r="123">
       <c r="A123" s="0">
-        <v>85.509937169312195</v>
+        <v>138.05430311671483</v>
       </c>
       <c r="B123" s="0">
-        <v>12</v>
+        <v>10.533333333333333</v>
       </c>
       <c r="C123" s="0">
         <v>2.9922</v>
@@ -2156,10 +2156,10 @@
     </row>
     <row r="124">
       <c r="A124" s="0">
-        <v>86.210838293650809</v>
+        <v>139.18589576521248</v>
       </c>
       <c r="B124" s="0">
-        <v>12</v>
+        <v>10.699999999999999</v>
       </c>
       <c r="C124" s="0">
         <v>2.9464999999999999</v>
@@ -2173,10 +2173,10 @@
     </row>
     <row r="125">
       <c r="A125" s="0">
-        <v>86.911739417989438</v>
+        <v>140.31748841371015</v>
       </c>
       <c r="B125" s="0">
-        <v>12</v>
+        <v>10.833333333333332</v>
       </c>
       <c r="C125" s="0">
         <v>2.8593000000000002</v>
@@ -2190,10 +2190,10 @@
     </row>
     <row r="126">
       <c r="A126" s="0">
-        <v>87.612640542328066</v>
+        <v>141.44908106220782</v>
       </c>
       <c r="B126" s="0">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C126" s="0">
         <v>2.7650999999999999</v>
@@ -2207,10 +2207,10 @@
     </row>
     <row r="127">
       <c r="A127" s="0">
-        <v>88.31354166666668</v>
+        <v>142.5806737107055</v>
       </c>
       <c r="B127" s="0">
-        <v>12</v>
+        <v>11.133333333333333</v>
       </c>
       <c r="C127" s="0">
         <v>2.6997</v>
@@ -2224,10 +2224,10 @@
     </row>
     <row r="128">
       <c r="A128" s="0">
-        <v>89.014442791005308</v>
+        <v>143.71226635920314</v>
       </c>
       <c r="B128" s="0">
-        <v>12</v>
+        <v>11.300000000000001</v>
       </c>
       <c r="C128" s="0">
         <v>2.6198999999999999</v>
@@ -2241,10 +2241,10 @@
     </row>
     <row r="129">
       <c r="A129" s="0">
-        <v>89.715343915343936</v>
+        <v>144.84385900770081</v>
       </c>
       <c r="B129" s="0">
-        <v>12</v>
+        <v>11.433333333333334</v>
       </c>
       <c r="C129" s="0">
         <v>2.5204</v>
@@ -2258,10 +2258,10 @@
     </row>
     <row r="130">
       <c r="A130" s="0">
-        <v>90.416245039682565</v>
+        <v>145.97545165619849</v>
       </c>
       <c r="B130" s="0">
-        <v>12</v>
+        <v>11.566666666666666</v>
       </c>
       <c r="C130" s="0">
         <v>2.4144999999999999</v>
@@ -2275,10 +2275,10 @@
     </row>
     <row r="131">
       <c r="A131" s="0">
-        <v>91.117146164021179</v>
+        <v>147.10704430469613</v>
       </c>
       <c r="B131" s="0">
-        <v>12</v>
+        <v>11.733333333333334</v>
       </c>
       <c r="C131" s="0">
         <v>2.3246000000000002</v>
@@ -2292,10 +2292,10 @@
     </row>
     <row r="132">
       <c r="A132" s="0">
-        <v>91.818047288359821</v>
+        <v>148.2386369531938</v>
       </c>
       <c r="B132" s="0">
-        <v>12</v>
+        <v>11.866666666666667</v>
       </c>
       <c r="C132" s="0">
         <v>2.2181000000000002</v>
@@ -2309,7 +2309,7 @@
     </row>
     <row r="133">
       <c r="A133" s="0">
-        <v>92.518948412698435</v>
+        <v>149.37022960169145</v>
       </c>
       <c r="B133" s="0">
         <v>12</v>
@@ -2326,7 +2326,7 @@
     </row>
     <row r="134">
       <c r="A134" s="0">
-        <v>93.219849537037064</v>
+        <v>150.50182225018912</v>
       </c>
       <c r="B134" s="0">
         <v>12</v>
@@ -2343,7 +2343,7 @@
     </row>
     <row r="135">
       <c r="A135" s="0">
-        <v>93.920750661375678</v>
+        <v>151.63341489868677</v>
       </c>
       <c r="B135" s="0">
         <v>12</v>
@@ -2360,7 +2360,7 @@
     </row>
     <row r="136">
       <c r="A136" s="0">
-        <v>94.621651785714306</v>
+        <v>152.76500754718444</v>
       </c>
       <c r="B136" s="0">
         <v>12</v>
@@ -2377,7 +2377,7 @@
     </row>
     <row r="137">
       <c r="A137" s="0">
-        <v>95.32255291005292</v>
+        <v>153.89660019568211</v>
       </c>
       <c r="B137" s="0">
         <v>12</v>
@@ -2394,7 +2394,7 @@
     </row>
     <row r="138">
       <c r="A138" s="0">
-        <v>96.023454034391563</v>
+        <v>155.02819284417976</v>
       </c>
       <c r="B138" s="0">
         <v>12</v>
@@ -2411,7 +2411,7 @@
     </row>
     <row r="139">
       <c r="A139" s="0">
-        <v>96.724355158730177</v>
+        <v>156.15978549267743</v>
       </c>
       <c r="B139" s="0">
         <v>12</v>
@@ -2428,7 +2428,7 @@
     </row>
     <row r="140">
       <c r="A140" s="0">
-        <v>97.425256283068805</v>
+        <v>157.2913781411751</v>
       </c>
       <c r="B140" s="0">
         <v>12</v>
@@ -2445,7 +2445,7 @@
     </row>
     <row r="141">
       <c r="A141" s="0">
-        <v>98.126157407407419</v>
+        <v>158.42297078967277</v>
       </c>
       <c r="B141" s="0">
         <v>12</v>
@@ -2462,7 +2462,7 @@
     </row>
     <row r="142">
       <c r="A142" s="0">
-        <v>98.827058531746061</v>
+        <v>159.55456343817042</v>
       </c>
       <c r="B142" s="0">
         <v>12</v>
@@ -2479,7 +2479,7 @@
     </row>
     <row r="143">
       <c r="A143" s="0">
-        <v>99.527959656084676</v>
+        <v>160.68615608666809</v>
       </c>
       <c r="B143" s="0">
         <v>12</v>
@@ -2496,7 +2496,7 @@
     </row>
     <row r="144">
       <c r="A144" s="0">
-        <v>100.2288607804233</v>
+        <v>161.81774873516576</v>
       </c>
       <c r="B144" s="0">
         <v>12</v>
@@ -2513,7 +2513,7 @@
     </row>
     <row r="145">
       <c r="A145" s="0">
-        <v>100.92976190476192</v>
+        <v>162.94934138366341</v>
       </c>
       <c r="B145" s="0">
         <v>12</v>
@@ -2530,7 +2530,7 @@
     </row>
     <row r="146">
       <c r="A146" s="0">
-        <v>101.63066302910055</v>
+        <v>164.08093403216105</v>
       </c>
       <c r="B146" s="0">
         <v>12</v>
@@ -2547,7 +2547,7 @@
     </row>
     <row r="147">
       <c r="A147" s="0">
-        <v>102.33156415343919</v>
+        <v>165.21252668065873</v>
       </c>
       <c r="B147" s="0">
         <v>12</v>
@@ -2564,7 +2564,7 @@
     </row>
     <row r="148">
       <c r="A148" s="0">
-        <v>103.0324652777778</v>
+        <v>166.3441193291564</v>
       </c>
       <c r="B148" s="0">
         <v>12</v>
@@ -2581,7 +2581,7 @@
     </row>
     <row r="149">
       <c r="A149" s="0">
-        <v>103.73336640211643</v>
+        <v>167.47571197765404</v>
       </c>
       <c r="B149" s="0">
         <v>12</v>
@@ -2598,7 +2598,7 @@
     </row>
     <row r="150">
       <c r="A150" s="0">
-        <v>104.43426752645505</v>
+        <v>168.60730462615172</v>
       </c>
       <c r="B150" s="0">
         <v>12</v>
@@ -2615,7 +2615,7 @@
     </row>
     <row r="151">
       <c r="A151" s="0">
-        <v>105.13516865079367</v>
+        <v>169.73889727464939</v>
       </c>
       <c r="B151" s="0">
         <v>12</v>
@@ -2632,7 +2632,7 @@
     </row>
     <row r="152">
       <c r="A152" s="0">
-        <v>105.83606977513229</v>
+        <v>170.87048992314706</v>
       </c>
       <c r="B152" s="0">
         <v>12</v>
@@ -2649,7 +2649,7 @@
     </row>
     <row r="153">
       <c r="A153" s="0">
-        <v>106.53697089947093</v>
+        <v>172.00208257164471</v>
       </c>
       <c r="B153" s="0">
         <v>12</v>
@@ -2666,7 +2666,7 @@
     </row>
     <row r="154">
       <c r="A154" s="0">
-        <v>107.23787202380954</v>
+        <v>173.13367522014238</v>
       </c>
       <c r="B154" s="0">
         <v>12</v>
@@ -2683,7 +2683,7 @@
     </row>
     <row r="155">
       <c r="A155" s="0">
-        <v>107.93877314814817</v>
+        <v>174.26526786864005</v>
       </c>
       <c r="B155" s="0">
         <v>12</v>
@@ -2700,7 +2700,7 @@
     </row>
     <row r="156">
       <c r="A156" s="0">
-        <v>108.63967427248679</v>
+        <v>175.3968605171377</v>
       </c>
       <c r="B156" s="0">
         <v>12</v>
@@ -2717,7 +2717,7 @@
     </row>
     <row r="157">
       <c r="A157" s="0">
-        <v>109.34057539682543</v>
+        <v>176.52845316563537</v>
       </c>
       <c r="B157" s="0">
         <v>12</v>
@@ -2734,7 +2734,7 @@
     </row>
     <row r="158">
       <c r="A158" s="0">
-        <v>110.04147652116404</v>
+        <v>177.66004581413301</v>
       </c>
       <c r="B158" s="0">
         <v>12</v>
@@ -2751,7 +2751,7 @@
     </row>
     <row r="159">
       <c r="A159" s="0">
-        <v>110.74237764550267</v>
+        <v>178.79163846263069</v>
       </c>
       <c r="B159" s="0">
         <v>12</v>
@@ -2768,7 +2768,7 @@
     </row>
     <row r="160">
       <c r="A160" s="0">
-        <v>111.44327876984129</v>
+        <v>179.92323111112833</v>
       </c>
       <c r="B160" s="0">
         <v>12</v>
@@ -2785,7 +2785,7 @@
     </row>
     <row r="161">
       <c r="A161" s="0">
-        <v>112.14417989417991</v>
+        <v>181.054823759626</v>
       </c>
       <c r="B161" s="0">
         <v>12</v>
@@ -2802,7 +2802,7 @@
     </row>
     <row r="162">
       <c r="A162" s="0">
-        <v>112.84508101851856</v>
+        <v>182.18641640812368</v>
       </c>
       <c r="B162" s="0">
         <v>12</v>
@@ -2819,7 +2819,7 @@
     </row>
     <row r="163">
       <c r="A163" s="0">
-        <v>113.54598214285717</v>
+        <v>183.31800905662132</v>
       </c>
       <c r="B163" s="0">
         <v>12</v>
@@ -2836,7 +2836,7 @@
     </row>
     <row r="164">
       <c r="A164" s="0">
-        <v>114.2468832671958</v>
+        <v>184.44960170511899</v>
       </c>
       <c r="B164" s="0">
         <v>12</v>
@@ -2853,7 +2853,7 @@
     </row>
     <row r="165">
       <c r="A165" s="0">
-        <v>114.94778439153441</v>
+        <v>185.58119435361667</v>
       </c>
       <c r="B165" s="0">
         <v>12</v>
@@ -2870,7 +2870,7 @@
     </row>
     <row r="166">
       <c r="A166" s="0">
-        <v>115.64868551587304</v>
+        <v>186.71278700211434</v>
       </c>
       <c r="B166" s="0">
         <v>12</v>
@@ -2887,7 +2887,7 @@
     </row>
     <row r="167">
       <c r="A167" s="0">
-        <v>116.34958664021165</v>
+        <v>187.84437965061198</v>
       </c>
       <c r="B167" s="0">
         <v>12</v>
@@ -2904,7 +2904,7 @@
     </row>
     <row r="168">
       <c r="A168" s="0">
-        <v>117.0504877645503</v>
+        <v>188.97597229910966</v>
       </c>
       <c r="B168" s="0">
         <v>12</v>
@@ -2921,7 +2921,7 @@
     </row>
     <row r="169">
       <c r="A169" s="0">
-        <v>117.75138888888891</v>
+        <v>190.10756494760733</v>
       </c>
       <c r="B169" s="0">
         <v>12</v>
@@ -2938,7 +2938,7 @@
     </row>
     <row r="170">
       <c r="A170" s="0">
-        <v>118.45229001322754</v>
+        <v>191.23915759610497</v>
       </c>
       <c r="B170" s="0">
         <v>12</v>
@@ -2955,7 +2955,7 @@
     </row>
     <row r="171">
       <c r="A171" s="0">
-        <v>119.15319113756615</v>
+        <v>192.37075024460262</v>
       </c>
       <c r="B171" s="0">
         <v>12</v>
@@ -2972,7 +2972,7 @@
     </row>
     <row r="172">
       <c r="A172" s="0">
-        <v>119.8540922619048</v>
+        <v>193.50234289310029</v>
       </c>
       <c r="B172" s="0">
         <v>12</v>
@@ -2989,7 +2989,7 @@
     </row>
     <row r="173">
       <c r="A173" s="0">
-        <v>120.55499338624341</v>
+        <v>194.63393554159796</v>
       </c>
       <c r="B173" s="0">
         <v>12</v>
@@ -3006,7 +3006,7 @@
     </row>
     <row r="174">
       <c r="A174" s="0">
-        <v>121.25589451058204</v>
+        <v>195.76552819009561</v>
       </c>
       <c r="B174" s="0">
         <v>12</v>
@@ -3023,7 +3023,7 @@
     </row>
     <row r="175">
       <c r="A175" s="0">
-        <v>121.95679563492065</v>
+        <v>196.89712083859328</v>
       </c>
       <c r="B175" s="0">
         <v>12</v>
@@ -3040,7 +3040,7 @@
     </row>
     <row r="176">
       <c r="A176" s="0">
-        <v>122.65769675925928</v>
+        <v>198.02871348709095</v>
       </c>
       <c r="B176" s="0">
         <v>12</v>
@@ -3057,7 +3057,7 @@
     </row>
     <row r="177">
       <c r="A177" s="0">
-        <v>123.35859788359792</v>
+        <v>199.1603061355886</v>
       </c>
       <c r="B177" s="0">
         <v>12</v>
@@ -3074,7 +3074,7 @@
     </row>
     <row r="178">
       <c r="A178" s="0">
-        <v>124.05949900793654</v>
+        <v>200.29189878408627</v>
       </c>
       <c r="B178" s="0">
         <v>12</v>
@@ -3091,7 +3091,7 @@
     </row>
     <row r="179">
       <c r="A179" s="0">
-        <v>124.76040013227517</v>
+        <v>201.42349143258394</v>
       </c>
       <c r="B179" s="0">
         <v>12</v>
@@ -3108,7 +3108,7 @@
     </row>
     <row r="180">
       <c r="A180" s="0">
-        <v>125.46130125661378</v>
+        <v>202.55508408108162</v>
       </c>
       <c r="B180" s="0">
         <v>12</v>
@@ -3125,7 +3125,7 @@
     </row>
     <row r="181">
       <c r="A181" s="0">
-        <v>126.16220238095242</v>
+        <v>203.68667672957926</v>
       </c>
       <c r="B181" s="0">
         <v>12</v>
@@ -3142,10 +3142,10 @@
     </row>
     <row r="182">
       <c r="A182" s="0">
-        <v>126.86310350529104</v>
+        <v>204.81826937807693</v>
       </c>
       <c r="B182" s="0">
-        <v>11.970315398886827</v>
+        <v>11.946607341490544</v>
       </c>
       <c r="C182" s="0">
         <v>-0.78183000000000002</v>
@@ -3159,10 +3159,10 @@
     </row>
     <row r="183">
       <c r="A183" s="0">
-        <v>127.56400462962966</v>
+        <v>205.94986202657458</v>
       </c>
       <c r="B183" s="0">
-        <v>11.940630797773656</v>
+        <v>11.893214682981091</v>
       </c>
       <c r="C183" s="0">
         <v>-0.79227999999999998</v>
@@ -3176,10 +3176,10 @@
     </row>
     <row r="184">
       <c r="A184" s="0">
-        <v>128.26490575396826</v>
+        <v>207.08145467507225</v>
       </c>
       <c r="B184" s="0">
-        <v>11.903525046382189</v>
+        <v>11.826473859844272</v>
       </c>
       <c r="C184" s="0">
         <v>-0.79059000000000001</v>
@@ -3193,10 +3193,10 @@
     </row>
     <row r="185">
       <c r="A185" s="0">
-        <v>128.96580687830692</v>
+        <v>208.2130473235699</v>
       </c>
       <c r="B185" s="0">
-        <v>11.873840445269018</v>
+        <v>11.773081201334817</v>
       </c>
       <c r="C185" s="0">
         <v>-0.80498000000000003</v>
@@ -3210,10 +3210,10 @@
     </row>
     <row r="186">
       <c r="A186" s="0">
-        <v>129.66670800264552</v>
+        <v>209.34463997206757</v>
       </c>
       <c r="B186" s="0">
-        <v>11.844155844155845</v>
+        <v>11.719688542825361</v>
       </c>
       <c r="C186" s="0">
         <v>-0.81388000000000005</v>
@@ -3227,10 +3227,10 @@
     </row>
     <row r="187">
       <c r="A187" s="0">
-        <v>130.36760912698415</v>
+        <v>210.47623262056524</v>
       </c>
       <c r="B187" s="0">
-        <v>11.814471243042671</v>
+        <v>11.666295884315907</v>
       </c>
       <c r="C187" s="0">
         <v>-0.82108000000000003</v>
@@ -3244,10 +3244,10 @@
     </row>
     <row r="188">
       <c r="A188" s="0">
-        <v>131.06851025132278</v>
+        <v>211.60782526906289</v>
       </c>
       <c r="B188" s="0">
-        <v>11.784786641929498</v>
+        <v>11.599555061179087</v>
       </c>
       <c r="C188" s="0">
         <v>-0.85433999999999999</v>
@@ -3261,10 +3261,10 @@
     </row>
     <row r="189">
       <c r="A189" s="0">
-        <v>131.76941137566141</v>
+        <v>212.73941791756056</v>
       </c>
       <c r="B189" s="0">
-        <v>11.747680890538033</v>
+        <v>11.546162402669633</v>
       </c>
       <c r="C189" s="0">
         <v>-0.87036999999999998</v>
@@ -3278,10 +3278,10 @@
     </row>
     <row r="190">
       <c r="A190" s="0">
-        <v>132.47031250000003</v>
+        <v>213.87101056605823</v>
       </c>
       <c r="B190" s="0">
-        <v>11.71799628942486</v>
+        <v>11.492769744160178</v>
       </c>
       <c r="C190" s="0">
         <v>-0.88980000000000004</v>
@@ -3295,10 +3295,10 @@
     </row>
     <row r="191">
       <c r="A191" s="0">
-        <v>133.17121362433866</v>
+        <v>215.0026032145559</v>
       </c>
       <c r="B191" s="0">
-        <v>11.688311688311689</v>
+        <v>11.426028921023359</v>
       </c>
       <c r="C191" s="0">
         <v>-0.91710999999999998</v>
@@ -3312,10 +3312,10 @@
     </row>
     <row r="192">
       <c r="A192" s="0">
-        <v>133.87211474867726</v>
+        <v>216.13419586305355</v>
       </c>
       <c r="B192" s="0">
-        <v>11.658627087198516</v>
+        <v>11.372636262513904</v>
       </c>
       <c r="C192" s="0">
         <v>-0.94099999999999995</v>
@@ -3329,10 +3329,10 @@
     </row>
     <row r="193">
       <c r="A193" s="0">
-        <v>134.57301587301589</v>
+        <v>217.26578851155122</v>
       </c>
       <c r="B193" s="0">
-        <v>11.621521335807049</v>
+        <v>11.31924360400445</v>
       </c>
       <c r="C193" s="0">
         <v>-0.95908000000000004</v>
@@ -3346,10 +3346,10 @@
     </row>
     <row r="194">
       <c r="A194" s="0">
-        <v>135.27391699735455</v>
+        <v>218.39738116004889</v>
       </c>
       <c r="B194" s="0">
-        <v>11.591836734693878</v>
+        <v>11.25250278086763</v>
       </c>
       <c r="C194" s="0">
         <v>-0.97258999999999995</v>
@@ -3363,10 +3363,10 @@
     </row>
     <row r="195">
       <c r="A195" s="0">
-        <v>135.97481812169315</v>
+        <v>219.52897380854654</v>
       </c>
       <c r="B195" s="0">
-        <v>11.562152133580705</v>
+        <v>11.199110122358176</v>
       </c>
       <c r="C195" s="0">
         <v>-0.99770000000000003</v>
@@ -3380,10 +3380,10 @@
     </row>
     <row r="196">
       <c r="A196" s="0">
-        <v>136.67571924603178</v>
+        <v>220.66056645704418</v>
       </c>
       <c r="B196" s="0">
-        <v>11.52504638218924</v>
+        <v>11.132369299221358</v>
       </c>
       <c r="C196" s="0">
         <v>-1.0021</v>
@@ -3397,10 +3397,10 @@
     </row>
     <row r="197">
       <c r="A197" s="0">
-        <v>137.3766203703704</v>
+        <v>221.79215910554186</v>
       </c>
       <c r="B197" s="0">
-        <v>11.495361781076067</v>
+        <v>11.078976640711902</v>
       </c>
       <c r="C197" s="0">
         <v>-1.0205</v>
@@ -3414,10 +3414,10 @@
     </row>
     <row r="198">
       <c r="A198" s="0">
-        <v>138.07752149470903</v>
+        <v>222.92375175403953</v>
       </c>
       <c r="B198" s="0">
-        <v>11.465677179962894</v>
+        <v>11.012235817575084</v>
       </c>
       <c r="C198" s="0">
         <v>-1.03</v>
@@ -3431,10 +3431,10 @@
     </row>
     <row r="199">
       <c r="A199" s="0">
-        <v>138.77842261904763</v>
+        <v>224.05534440253717</v>
       </c>
       <c r="B199" s="0">
-        <v>11.428571428571429</v>
+        <v>10.958843159065628</v>
       </c>
       <c r="C199" s="0">
         <v>-1.0475000000000001</v>
@@ -3448,10 +3448,10 @@
     </row>
     <row r="200">
       <c r="A200" s="0">
-        <v>139.47932374338629</v>
+        <v>225.18693705103485</v>
       </c>
       <c r="B200" s="0">
-        <v>11.398886827458256</v>
+        <v>10.89210233592881</v>
       </c>
       <c r="C200" s="0">
         <v>-1.0488</v>
@@ -3465,10 +3465,10 @@
     </row>
     <row r="201">
       <c r="A201" s="0">
-        <v>140.18022486772489</v>
+        <v>226.31852969953252</v>
       </c>
       <c r="B201" s="0">
-        <v>11.361781076066791</v>
+        <v>10.825361512791991</v>
       </c>
       <c r="C201" s="0">
         <v>-1.0607</v>
@@ -3482,10 +3482,10 @@
     </row>
     <row r="202">
       <c r="A202" s="0">
-        <v>140.88112599206352</v>
+        <v>227.45012234803016</v>
       </c>
       <c r="B202" s="0">
-        <v>11.332096474953618</v>
+        <v>10.771968854282536</v>
       </c>
       <c r="C202" s="0">
         <v>-1.0603</v>
@@ -3499,10 +3499,10 @@
     </row>
     <row r="203">
       <c r="A203" s="0">
-        <v>141.58202711640214</v>
+        <v>228.58171499652786</v>
       </c>
       <c r="B203" s="0">
-        <v>11.302411873840445</v>
+        <v>10.705228031145717</v>
       </c>
       <c r="C203" s="0">
         <v>-1.0762</v>
@@ -3516,10 +3516,10 @@
     </row>
     <row r="204">
       <c r="A204" s="0">
-        <v>142.28292824074077</v>
+        <v>229.71330764502551</v>
       </c>
       <c r="B204" s="0">
-        <v>11.26530612244898</v>
+        <v>10.651835372636263</v>
       </c>
       <c r="C204" s="0">
         <v>-1.0899000000000001</v>
@@ -3533,10 +3533,10 @@
     </row>
     <row r="205">
       <c r="A205" s="0">
-        <v>142.9838293650794</v>
+        <v>230.84490029352315</v>
       </c>
       <c r="B205" s="0">
-        <v>11.235621521335807</v>
+        <v>10.585094549499445</v>
       </c>
       <c r="C205" s="0">
         <v>-1.0865</v>
@@ -3550,10 +3550,10 @@
     </row>
     <row r="206">
       <c r="A206" s="0">
-        <v>143.68473048941803</v>
+        <v>231.97649294202085</v>
       </c>
       <c r="B206" s="0">
-        <v>11.198515769944342</v>
+        <v>10.518353726362625</v>
       </c>
       <c r="C206" s="0">
         <v>-1.1233</v>
@@ -3567,10 +3567,10 @@
     </row>
     <row r="207">
       <c r="A207" s="0">
-        <v>144.38563161375663</v>
+        <v>233.1080855905185</v>
       </c>
       <c r="B207" s="0">
-        <v>11.168831168831169</v>
+        <v>10.451612903225806</v>
       </c>
       <c r="C207" s="0">
         <v>-1.1056999999999999</v>
@@ -3584,10 +3584,10 @@
     </row>
     <row r="208">
       <c r="A208" s="0">
-        <v>145.08653273809526</v>
+        <v>234.23967823901614</v>
       </c>
       <c r="B208" s="0">
-        <v>11.131725417439704</v>
+        <v>10.384872080088988</v>
       </c>
       <c r="C208" s="0">
         <v>-1.1309</v>
@@ -3601,10 +3601,10 @@
     </row>
     <row r="209">
       <c r="A209" s="0">
-        <v>145.78743386243389</v>
+        <v>235.37127088751382</v>
       </c>
       <c r="B209" s="0">
-        <v>11.102040816326531</v>
+        <v>10.331479421579534</v>
       </c>
       <c r="C209" s="0">
         <v>-1.1516</v>
@@ -3618,10 +3618,10 @@
     </row>
     <row r="210">
       <c r="A210" s="0">
-        <v>146.48833498677251</v>
+        <v>236.50286353601146</v>
       </c>
       <c r="B210" s="0">
-        <v>11.064935064935066</v>
+        <v>10.264738598442714</v>
       </c>
       <c r="C210" s="0">
         <v>-1.1333</v>
@@ -3635,10 +3635,10 @@
     </row>
     <row r="211">
       <c r="A211" s="0">
-        <v>147.18923611111114</v>
+        <v>237.63445618450911</v>
       </c>
       <c r="B211" s="0">
-        <v>11.035250463821892</v>
+        <v>10.197997775305895</v>
       </c>
       <c r="C211" s="0">
         <v>-1.1306</v>
@@ -3652,10 +3652,10 @@
     </row>
     <row r="212">
       <c r="A212" s="0">
-        <v>147.89013723544977</v>
+        <v>238.76604883300681</v>
       </c>
       <c r="B212" s="0">
-        <v>10.998144712430427</v>
+        <v>10.131256952169077</v>
       </c>
       <c r="C212" s="0">
         <v>-1.1343000000000001</v>
@@ -3669,10 +3669,10 @@
     </row>
     <row r="213">
       <c r="A213" s="0">
-        <v>148.5910383597884</v>
+        <v>239.89764148150445</v>
       </c>
       <c r="B213" s="0">
-        <v>10.968460111317254</v>
+        <v>10.064516129032258</v>
       </c>
       <c r="C213" s="0">
         <v>-1.1496</v>
@@ -3686,10 +3686,10 @@
     </row>
     <row r="214">
       <c r="A214" s="0">
-        <v>149.291939484127</v>
+        <v>241.02923413000215</v>
       </c>
       <c r="B214" s="0">
-        <v>10.931354359925788</v>
+        <v>9.9977753058954395</v>
       </c>
       <c r="C214" s="0">
         <v>-1.2184999999999999</v>
@@ -3703,10 +3703,10 @@
     </row>
     <row r="215">
       <c r="A215" s="0">
-        <v>149.99284060846566</v>
+        <v>242.1608267784998</v>
       </c>
       <c r="B215" s="0">
-        <v>10.901669758812616</v>
+        <v>9.931034482758621</v>
       </c>
       <c r="C215" s="0">
         <v>-1.294</v>
@@ -3720,10 +3720,10 @@
     </row>
     <row r="216">
       <c r="A216" s="0">
-        <v>150.69374173280426</v>
+        <v>243.29241942699744</v>
       </c>
       <c r="B216" s="0">
-        <v>10.864564007421151</v>
+        <v>9.8642936596218025</v>
       </c>
       <c r="C216" s="0">
         <v>-1.3495999999999999</v>
@@ -3737,10 +3737,10 @@
     </row>
     <row r="217">
       <c r="A217" s="0">
-        <v>151.39464285714288</v>
+        <v>244.42401207549514</v>
       </c>
       <c r="B217" s="0">
-        <v>10.834879406307978</v>
+        <v>9.7975528364849822</v>
       </c>
       <c r="C217" s="0">
         <v>-1.4133</v>
@@ -3754,10 +3754,10 @@
     </row>
     <row r="218">
       <c r="A218" s="0">
-        <v>152.09554398148151</v>
+        <v>245.55560472399279</v>
       </c>
       <c r="B218" s="0">
-        <v>10.797773654916512</v>
+        <v>9.7308120133481637</v>
       </c>
       <c r="C218" s="0">
         <v>-1.4789000000000001</v>
@@ -3771,10 +3771,10 @@
     </row>
     <row r="219">
       <c r="A219" s="0">
-        <v>152.79644510582014</v>
+        <v>246.68719737249043</v>
       </c>
       <c r="B219" s="0">
-        <v>10.760667903525047</v>
+        <v>9.6640711902113452</v>
       </c>
       <c r="C219" s="0">
         <v>-1.4778</v>
@@ -3788,10 +3788,10 @@
     </row>
     <row r="220">
       <c r="A220" s="0">
-        <v>153.49734623015877</v>
+        <v>247.8187900209881</v>
       </c>
       <c r="B220" s="0">
-        <v>10.730983302411873</v>
+        <v>9.5839822024471637</v>
       </c>
       <c r="C220" s="0">
         <v>-1.4619</v>
@@ -3805,10 +3805,10 @@
     </row>
     <row r="221">
       <c r="A221" s="0">
-        <v>154.1982473544974</v>
+        <v>248.95038266948575</v>
       </c>
       <c r="B221" s="0">
-        <v>10.693877551020408</v>
+        <v>9.5172413793103452</v>
       </c>
       <c r="C221" s="0">
         <v>-1.4065000000000001</v>
@@ -3822,10 +3822,10 @@
     </row>
     <row r="222">
       <c r="A222" s="0">
-        <v>154.899148478836</v>
+        <v>250.08197531798339</v>
       </c>
       <c r="B222" s="0">
-        <v>10.656771799628942</v>
+        <v>9.4505005561735267</v>
       </c>
       <c r="C222" s="0">
         <v>-1.3362000000000001</v>
@@ -3839,10 +3839,10 @@
     </row>
     <row r="223">
       <c r="A223" s="0">
-        <v>155.60004960317463</v>
+        <v>251.21356796648109</v>
       </c>
       <c r="B223" s="0">
-        <v>10.62708719851577</v>
+        <v>9.3837597330367082</v>
       </c>
       <c r="C223" s="0">
         <v>-1.2712000000000001</v>
@@ -3856,10 +3856,10 @@
     </row>
     <row r="224">
       <c r="A224" s="0">
-        <v>156.30095072751325</v>
+        <v>252.34516061497874</v>
       </c>
       <c r="B224" s="0">
-        <v>10.589981447124304</v>
+        <v>9.3036707452725249</v>
       </c>
       <c r="C224" s="0">
         <v>-1.2374000000000001</v>
@@ -3873,10 +3873,10 @@
     </row>
     <row r="225">
       <c r="A225" s="0">
-        <v>157.00185185185188</v>
+        <v>253.47675326347638</v>
       </c>
       <c r="B225" s="0">
-        <v>10.552875695732839</v>
+        <v>9.2369299221357064</v>
       </c>
       <c r="C225" s="0">
         <v>-1.1685000000000001</v>
@@ -3890,10 +3890,10 @@
     </row>
     <row r="226">
       <c r="A226" s="0">
-        <v>157.70275297619051</v>
+        <v>254.60834591197408</v>
       </c>
       <c r="B226" s="0">
-        <v>10.515769944341374</v>
+        <v>9.1701890989988879</v>
       </c>
       <c r="C226" s="0">
         <v>-1.0986</v>
@@ -3907,10 +3907,10 @@
     </row>
     <row r="227">
       <c r="A227" s="0">
-        <v>158.40365410052914</v>
+        <v>255.73993856047173</v>
       </c>
       <c r="B227" s="0">
-        <v>10.486085343228201</v>
+        <v>9.0901001112347046</v>
       </c>
       <c r="C227" s="0">
         <v>-1.0041</v>
@@ -3924,10 +3924,10 @@
     </row>
     <row r="228">
       <c r="A228" s="0">
-        <v>159.10455522486777</v>
+        <v>256.87153120896943</v>
       </c>
       <c r="B228" s="0">
-        <v>10.448979591836736</v>
+        <v>9.0233592880978861</v>
       </c>
       <c r="C228" s="0">
         <v>-0.92332000000000003</v>
@@ -3941,10 +3941,10 @@
     </row>
     <row r="229">
       <c r="A229" s="0">
-        <v>159.80545634920639</v>
+        <v>258.00312385746707</v>
       </c>
       <c r="B229" s="0">
-        <v>10.411873840445269</v>
+        <v>8.9432703003337046</v>
       </c>
       <c r="C229" s="0">
         <v>-0.88022999999999996</v>
@@ -3958,10 +3958,10 @@
     </row>
     <row r="230">
       <c r="A230" s="0">
-        <v>160.50635747354502</v>
+        <v>259.13471650596472</v>
       </c>
       <c r="B230" s="0">
-        <v>10.374768089053804</v>
+        <v>8.8631813125695214</v>
       </c>
       <c r="C230" s="0">
         <v>-0.91493000000000002</v>
@@ -3975,10 +3975,10 @@
     </row>
     <row r="231">
       <c r="A231" s="0">
-        <v>161.20725859788362</v>
+        <v>260.26630915446242</v>
       </c>
       <c r="B231" s="0">
-        <v>10.345083487940631</v>
+        <v>8.7964404894327028</v>
       </c>
       <c r="C231" s="0">
         <v>-0.99950000000000006</v>
@@ -3992,10 +3992,10 @@
     </row>
     <row r="232">
       <c r="A232" s="0">
-        <v>161.90815972222225</v>
+        <v>261.39790180296006</v>
       </c>
       <c r="B232" s="0">
-        <v>10.307977736549166</v>
+        <v>8.7163515016685196</v>
       </c>
       <c r="C232" s="0">
         <v>-1.0490999999999999</v>
@@ -4009,10 +4009,10 @@
     </row>
     <row r="233">
       <c r="A233" s="0">
-        <v>162.60906084656088</v>
+        <v>262.52949445145771</v>
       </c>
       <c r="B233" s="0">
-        <v>10.270871985157699</v>
+        <v>8.6362625139043381</v>
       </c>
       <c r="C233" s="0">
         <v>-1.1572</v>
@@ -4026,10 +4026,10 @@
     </row>
     <row r="234">
       <c r="A234" s="0">
-        <v>163.30996197089951</v>
+        <v>263.66108709995541</v>
       </c>
       <c r="B234" s="0">
-        <v>10.233766233766234</v>
+        <v>8.5695216907675196</v>
       </c>
       <c r="C234" s="0">
         <v>-1.2352000000000001</v>
@@ -4043,10 +4043,10 @@
     </row>
     <row r="235">
       <c r="A235" s="0">
-        <v>164.01086309523814</v>
+        <v>264.79267974845305</v>
       </c>
       <c r="B235" s="0">
-        <v>10.196660482374767</v>
+        <v>8.4894327030033381</v>
       </c>
       <c r="C235" s="0">
         <v>-1.2925</v>
@@ -4060,10 +4060,10 @@
     </row>
     <row r="236">
       <c r="A236" s="0">
-        <v>164.71176421957676</v>
+        <v>265.9242723969507</v>
       </c>
       <c r="B236" s="0">
-        <v>10.159554730983302</v>
+        <v>8.4093437152391548</v>
       </c>
       <c r="C236" s="0">
         <v>-1.2543</v>
@@ -4077,10 +4077,10 @@
     </row>
     <row r="237">
       <c r="A237" s="0">
-        <v>165.41266534391536</v>
+        <v>267.0558650454484</v>
       </c>
       <c r="B237" s="0">
-        <v>10.122448979591837</v>
+        <v>8.3292547274749715</v>
       </c>
       <c r="C237" s="0">
         <v>-1.2888999999999999</v>
@@ -4094,10 +4094,10 @@
     </row>
     <row r="238">
       <c r="A238" s="0">
-        <v>166.11356646825399</v>
+        <v>268.18745769394604</v>
       </c>
       <c r="B238" s="0">
-        <v>10.085343228200371</v>
+        <v>8.24916573971079</v>
       </c>
       <c r="C238" s="0">
         <v>-1.2423999999999999</v>
@@ -4111,10 +4111,10 @@
     </row>
     <row r="239">
       <c r="A239" s="0">
-        <v>166.81446759259262</v>
+        <v>269.31905034244369</v>
       </c>
       <c r="B239" s="0">
-        <v>10.048237476808906</v>
+        <v>8.1690767519466068</v>
       </c>
       <c r="C239" s="0">
         <v>-1.2007000000000001</v>
@@ -4128,10 +4128,10 @@
     </row>
     <row r="240">
       <c r="A240" s="0">
-        <v>167.51536871693125</v>
+        <v>270.45064299094133</v>
       </c>
       <c r="B240" s="0">
-        <v>10.011131725417441</v>
+        <v>8.0889877641824253</v>
       </c>
       <c r="C240" s="0">
         <v>-1.1524000000000001</v>
@@ -4145,10 +4145,10 @@
     </row>
     <row r="241">
       <c r="A241" s="0">
-        <v>168.21626984126988</v>
+        <v>271.58223563943898</v>
       </c>
       <c r="B241" s="0">
-        <v>9.9740259740259738</v>
+        <v>7.995550611790879</v>
       </c>
       <c r="C241" s="0">
         <v>-1.0710999999999999</v>
@@ -4162,10 +4162,10 @@
     </row>
     <row r="242">
       <c r="A242" s="0">
-        <v>168.91717096560851</v>
+        <v>272.71382828793668</v>
       </c>
       <c r="B242" s="0">
-        <v>9.9369202226345088</v>
+        <v>7.9154616240266966</v>
       </c>
       <c r="C242" s="0">
         <v>-1.0818000000000001</v>
@@ -4179,10 +4179,10 @@
     </row>
     <row r="243">
       <c r="A243" s="0">
-        <v>169.61807208994713</v>
+        <v>273.84542093643432</v>
       </c>
       <c r="B243" s="0">
-        <v>9.8998144712430438</v>
+        <v>7.8353726362625142</v>
       </c>
       <c r="C243" s="0">
         <v>-1.0683</v>
@@ -4196,10 +4196,10 @@
     </row>
     <row r="244">
       <c r="A244" s="0">
-        <v>170.31897321428576</v>
+        <v>274.97701358493197</v>
       </c>
       <c r="B244" s="0">
-        <v>9.862708719851577</v>
+        <v>7.741935483870968</v>
       </c>
       <c r="C244" s="0">
         <v>-1.0743</v>
@@ -4213,10 +4213,10 @@
     </row>
     <row r="245">
       <c r="A245" s="0">
-        <v>171.01987433862439</v>
+        <v>276.10860623342967</v>
       </c>
       <c r="B245" s="0">
-        <v>9.8256029684601121</v>
+        <v>7.6618464961067856</v>
       </c>
       <c r="C245" s="0">
         <v>-1.0607</v>
@@ -4230,10 +4230,10 @@
     </row>
     <row r="246">
       <c r="A246" s="0">
-        <v>171.72077546296299</v>
+        <v>277.24019888192731</v>
       </c>
       <c r="B246" s="0">
-        <v>9.7884972170686453</v>
+        <v>7.5684093437152393</v>
       </c>
       <c r="C246" s="0">
         <v>-1.0466</v>
@@ -4247,10 +4247,10 @@
     </row>
     <row r="247">
       <c r="A247" s="0">
-        <v>172.42167658730162</v>
+        <v>278.37179153042496</v>
       </c>
       <c r="B247" s="0">
-        <v>9.7513914656771803</v>
+        <v>7.4749721913236922</v>
       </c>
       <c r="C247" s="0">
         <v>-1.0468999999999999</v>
@@ -4264,10 +4264,10 @@
     </row>
     <row r="248">
       <c r="A248" s="0">
-        <v>173.12257771164025</v>
+        <v>279.50338417892266</v>
       </c>
       <c r="B248" s="0">
-        <v>9.7142857142857153</v>
+        <v>7.3948832035595107</v>
       </c>
       <c r="C248" s="0">
         <v>-1.0489999999999999</v>
@@ -4281,10 +4281,10 @@
     </row>
     <row r="249">
       <c r="A249" s="0">
-        <v>173.82347883597888</v>
+        <v>280.6349768274203</v>
       </c>
       <c r="B249" s="0">
-        <v>9.6771799628942485</v>
+        <v>7.3014460511679644</v>
       </c>
       <c r="C249" s="0">
         <v>-1.0506</v>
@@ -4298,10 +4298,10 @@
     </row>
     <row r="250">
       <c r="A250" s="0">
-        <v>174.5243799603175</v>
+        <v>281.76656947591795</v>
       </c>
       <c r="B250" s="0">
-        <v>9.6400742115027835</v>
+        <v>7.2080088987764181</v>
       </c>
       <c r="C250" s="0">
         <v>-1.0673999999999999</v>
@@ -4315,10 +4315,10 @@
     </row>
     <row r="251">
       <c r="A251" s="0">
-        <v>175.22528108465613</v>
+        <v>282.89816212441565</v>
       </c>
       <c r="B251" s="0">
-        <v>9.6029684601113168</v>
+        <v>7.1145717463848719</v>
       </c>
       <c r="C251" s="0">
         <v>-1.0704</v>
@@ -4332,10 +4332,10 @@
     </row>
     <row r="252">
       <c r="A252" s="0">
-        <v>175.92618220899473</v>
+        <v>284.02975477291329</v>
       </c>
       <c r="B252" s="0">
-        <v>9.5584415584415581</v>
+        <v>7.0211345939933256</v>
       </c>
       <c r="C252" s="0">
         <v>-1.0247999999999999</v>
@@ -4349,10 +4349,10 @@
     </row>
     <row r="253">
       <c r="A253" s="0">
-        <v>176.62708333333336</v>
+        <v>285.16134742141099</v>
       </c>
       <c r="B253" s="0">
-        <v>9.5213358070500931</v>
+        <v>6.9276974416017794</v>
       </c>
       <c r="C253" s="0">
         <v>-1.0326</v>
@@ -4366,10 +4366,10 @@
     </row>
     <row r="254">
       <c r="A254" s="0">
-        <v>177.32798445767199</v>
+        <v>286.29294006990864</v>
       </c>
       <c r="B254" s="0">
-        <v>9.4842300556586281</v>
+        <v>6.834260289210234</v>
       </c>
       <c r="C254" s="0">
         <v>-1.0105</v>
@@ -4383,10 +4383,10 @@
     </row>
     <row r="255">
       <c r="A255" s="0">
-        <v>178.02888558201062</v>
+        <v>287.42453271840628</v>
       </c>
       <c r="B255" s="0">
-        <v>9.4397031539888694</v>
+        <v>6.7274749721913238</v>
       </c>
       <c r="C255" s="0">
         <v>-0.99421999999999999</v>
@@ -4400,10 +4400,10 @@
     </row>
     <row r="256">
       <c r="A256" s="0">
-        <v>178.72978670634924</v>
+        <v>288.55612536690398</v>
       </c>
       <c r="B256" s="0">
-        <v>9.4025974025974026</v>
+        <v>6.6340378197997776</v>
       </c>
       <c r="C256" s="0">
         <v>-0.98019000000000001</v>
@@ -4417,10 +4417,10 @@
     </row>
     <row r="257">
       <c r="A257" s="0">
-        <v>179.43068783068787</v>
+        <v>289.68771801540163</v>
       </c>
       <c r="B257" s="0">
-        <v>9.3654916512059376</v>
+        <v>6.5272525027808674</v>
       </c>
       <c r="C257" s="0">
         <v>-0.93838999999999995</v>
@@ -4434,10 +4434,10 @@
     </row>
     <row r="258">
       <c r="A258" s="0">
-        <v>180.1315889550265</v>
+        <v>290.81931066389927</v>
       </c>
       <c r="B258" s="0">
-        <v>9.3283858998144709</v>
+        <v>6.4338153503893212</v>
       </c>
       <c r="C258" s="0">
         <v>-0.93408999999999998</v>
@@ -4451,10 +4451,10 @@
     </row>
     <row r="259">
       <c r="A259" s="0">
-        <v>180.83249007936513</v>
+        <v>291.95090331239697</v>
       </c>
       <c r="B259" s="0">
-        <v>9.2838589981447122</v>
+        <v>6.327030033370411</v>
       </c>
       <c r="C259" s="0">
         <v>-0.92035</v>
@@ -4468,10 +4468,10 @@
     </row>
     <row r="260">
       <c r="A260" s="0">
-        <v>181.53339120370376</v>
+        <v>293.08249596089462</v>
       </c>
       <c r="B260" s="0">
-        <v>9.2467532467532472</v>
+        <v>6.2202447163515018</v>
       </c>
       <c r="C260" s="0">
         <v>-0.91739999999999999</v>
@@ -4485,10 +4485,10 @@
     </row>
     <row r="261">
       <c r="A261" s="0">
-        <v>182.23429232804236</v>
+        <v>294.21408860939226</v>
       </c>
       <c r="B261" s="0">
-        <v>9.2022263450834885</v>
+        <v>6.1134593993325925</v>
       </c>
       <c r="C261" s="0">
         <v>-0.93491999999999997</v>
@@ -4502,10 +4502,10 @@
     </row>
     <row r="262">
       <c r="A262" s="0">
-        <v>182.93519345238099</v>
+        <v>295.34568125788996</v>
       </c>
       <c r="B262" s="0">
-        <v>9.1651205936920235</v>
+        <v>5.9933259176863185</v>
       </c>
       <c r="C262" s="0">
         <v>-0.91239000000000003</v>
@@ -4519,10 +4519,10 @@
     </row>
     <row r="263">
       <c r="A263" s="0">
-        <v>183.63609457671964</v>
+        <v>296.47727390638761</v>
       </c>
       <c r="B263" s="0">
-        <v>9.1205936920222648</v>
+        <v>5.8865406006674075</v>
       </c>
       <c r="C263" s="0">
         <v>-0.89661000000000002</v>
@@ -4536,10 +4536,10 @@
     </row>
     <row r="264">
       <c r="A264" s="0">
-        <v>184.33699570105821</v>
+        <v>297.60886655488525</v>
       </c>
       <c r="B264" s="0">
-        <v>9.083487940630798</v>
+        <v>5.7664071190211352</v>
       </c>
       <c r="C264" s="0">
         <v>-0.85046999999999995</v>
@@ -4553,10 +4553,10 @@
     </row>
     <row r="265">
       <c r="A265" s="0">
-        <v>185.03789682539687</v>
+        <v>298.7404592033829</v>
       </c>
       <c r="B265" s="0">
-        <v>9.0389610389610393</v>
+        <v>5.6596218020022242</v>
       </c>
       <c r="C265" s="0">
         <v>-0.81659000000000004</v>
@@ -4570,10 +4570,10 @@
     </row>
     <row r="266">
       <c r="A266" s="0">
-        <v>185.7387979497355</v>
+        <v>299.87205185188054</v>
       </c>
       <c r="B266" s="0">
-        <v>9.0018552875695725</v>
+        <v>5.5394883203559511</v>
       </c>
       <c r="C266" s="0">
         <v>-0.76624000000000003</v>
@@ -4587,10 +4587,10 @@
     </row>
     <row r="267">
       <c r="A267" s="0">
-        <v>186.43969907407413</v>
+        <v>301.00364450037824</v>
       </c>
       <c r="B267" s="0">
-        <v>8.9573283858998138</v>
+        <v>5.4193548387096779</v>
       </c>
       <c r="C267" s="0">
         <v>-0.78241000000000005</v>
@@ -4604,10 +4604,10 @@
     </row>
     <row r="268">
       <c r="A268" s="0">
-        <v>187.14060019841273</v>
+        <v>302.13523714887589</v>
       </c>
       <c r="B268" s="0">
-        <v>8.9202226345083488</v>
+        <v>5.28587319243604</v>
       </c>
       <c r="C268" s="0">
         <v>-0.77115999999999996</v>
@@ -4621,10 +4621,10 @@
     </row>
     <row r="269">
       <c r="A269" s="0">
-        <v>187.84150132275136</v>
+        <v>303.26682979737353</v>
       </c>
       <c r="B269" s="0">
-        <v>8.8756957328385901</v>
+        <v>5.165739710789766</v>
       </c>
       <c r="C269" s="0">
         <v>-0.73441999999999996</v>
@@ -4638,10 +4638,10 @@
     </row>
     <row r="270">
       <c r="A270" s="0">
-        <v>188.54240244708998</v>
+        <v>304.39842244587123</v>
       </c>
       <c r="B270" s="0">
-        <v>8.8385899814471252</v>
+        <v>5.032258064516129</v>
       </c>
       <c r="C270" s="0">
         <v>-0.71421999999999997</v>
@@ -4655,10 +4655,10 @@
     </row>
     <row r="271">
       <c r="A271" s="0">
-        <v>189.24330357142861</v>
+        <v>305.53001509436888</v>
       </c>
       <c r="B271" s="0">
-        <v>8.7940630797773665</v>
+        <v>4.898776418242492</v>
       </c>
       <c r="C271" s="0">
         <v>-0.70423000000000002</v>
@@ -4672,10 +4672,10 @@
     </row>
     <row r="272">
       <c r="A272" s="0">
-        <v>189.94420469576721</v>
+        <v>306.66160774286652</v>
       </c>
       <c r="B272" s="0">
-        <v>8.7495361781076078</v>
+        <v>4.7652947719688541</v>
       </c>
       <c r="C272" s="0">
         <v>-0.66556000000000004</v>
@@ -4689,10 +4689,10 @@
     </row>
     <row r="273">
       <c r="A273" s="0">
-        <v>190.64510582010584</v>
+        <v>307.79320039136422</v>
       </c>
       <c r="B273" s="0">
-        <v>8.7050092764378491</v>
+        <v>4.6184649610678532</v>
       </c>
       <c r="C273" s="0">
         <v>-0.63987000000000005</v>
@@ -4706,10 +4706,10 @@
     </row>
     <row r="274">
       <c r="A274" s="0">
-        <v>191.3460069444445</v>
+        <v>308.92479303986187</v>
       </c>
       <c r="B274" s="0">
-        <v>8.6679035250463823</v>
+        <v>4.4716351501668514</v>
       </c>
       <c r="C274" s="0">
         <v>-0.60604999999999998</v>
@@ -4723,10 +4723,10 @@
     </row>
     <row r="275">
       <c r="A275" s="0">
-        <v>192.04690806878313</v>
+        <v>310.05638568835951</v>
       </c>
       <c r="B275" s="0">
-        <v>8.6233766233766236</v>
+        <v>4.3248053392658505</v>
       </c>
       <c r="C275" s="0">
         <v>-0.59789000000000003</v>
@@ -4740,10 +4740,10 @@
     </row>
     <row r="276">
       <c r="A276" s="0">
-        <v>192.74780919312175</v>
+        <v>311.18797833685721</v>
       </c>
       <c r="B276" s="0">
-        <v>8.5788497217068649</v>
+        <v>4.1646273637374867</v>
       </c>
       <c r="C276" s="0">
         <v>-0.54781999999999997</v>
@@ -4757,10 +4757,10 @@
     </row>
     <row r="277">
       <c r="A277" s="0">
-        <v>193.44871031746035</v>
+        <v>312.31957098535486</v>
       </c>
       <c r="B277" s="0">
-        <v>8.5343228200371062</v>
+        <v>4.0044493882091219</v>
       </c>
       <c r="C277" s="0">
         <v>-0.49582999999999999</v>
@@ -4774,10 +4774,10 @@
     </row>
     <row r="278">
       <c r="A278" s="0">
-        <v>194.14961144179898</v>
+        <v>313.45116363385256</v>
       </c>
       <c r="B278" s="0">
-        <v>8.4972170686456394</v>
+        <v>3.8309232480533932</v>
       </c>
       <c r="C278" s="0">
         <v>-0.46034000000000003</v>
@@ -4791,10 +4791,10 @@
     </row>
     <row r="279">
       <c r="A279" s="0">
-        <v>194.85051256613761</v>
+        <v>314.5827562823502</v>
       </c>
       <c r="B279" s="0">
-        <v>8.4526901669758807</v>
+        <v>3.6573971078976655</v>
       </c>
       <c r="C279" s="0">
         <v>-0.41837999999999997</v>
@@ -4808,10 +4808,10 @@
     </row>
     <row r="280">
       <c r="A280" s="0">
-        <v>195.55141369047624</v>
+        <v>315.71434893084785</v>
       </c>
       <c r="B280" s="0">
-        <v>8.408163265306122</v>
+        <v>3.4571746384872082</v>
       </c>
       <c r="C280" s="0">
         <v>-0.36299999999999999</v>
@@ -4825,10 +4825,10 @@
     </row>
     <row r="281">
       <c r="A281" s="0">
-        <v>196.25231481481484</v>
+        <v>316.84594157934555</v>
       </c>
       <c r="B281" s="0">
-        <v>8.3487940630797777</v>
+        <v>3.1902113459399324</v>
       </c>
       <c r="C281" s="0">
         <v>-0.32049</v>
@@ -4842,10 +4842,10 @@
     </row>
     <row r="282">
       <c r="A282" s="0">
-        <v>196.95321593915347</v>
+        <v>317.97753422784319</v>
       </c>
       <c r="B282" s="0">
-        <v>8.304267161410019</v>
+        <v>3.0033370411568416</v>
       </c>
       <c r="C282" s="0">
         <v>-0.28726000000000002</v>
@@ -4859,10 +4859,10 @@
     </row>
     <row r="283">
       <c r="A283" s="0">
-        <v>197.65411706349212</v>
+        <v>319.10912687634084</v>
       </c>
       <c r="B283" s="0">
-        <v>8.2671614100185522</v>
+        <v>2.8031145717463861</v>
       </c>
       <c r="C283" s="0">
         <v>-0.25818000000000002</v>
@@ -4876,10 +4876,10 @@
     </row>
     <row r="284">
       <c r="A284" s="0">
-        <v>198.35501818783075</v>
+        <v>320.24071952483854</v>
       </c>
       <c r="B284" s="0">
-        <v>8.2300556586270872</v>
+        <v>2.5761957730812011</v>
       </c>
       <c r="C284" s="0">
         <v>-0.22964000000000001</v>
@@ -4893,10 +4893,10 @@
     </row>
     <row r="285">
       <c r="A285" s="0">
-        <v>199.05591931216935</v>
+        <v>321.37231217333618</v>
       </c>
       <c r="B285" s="0">
-        <v>8.1855287569573285</v>
+        <v>2.309232480533927</v>
       </c>
       <c r="C285" s="0">
         <v>-0.17512</v>
@@ -4910,10 +4910,10 @@
     </row>
     <row r="286">
       <c r="A286" s="0">
-        <v>199.75682043650798</v>
+        <v>322.50390482183383</v>
       </c>
       <c r="B286" s="0">
-        <v>8.1410018552875698</v>
+        <v>2.0022246941045605</v>
       </c>
       <c r="C286" s="0">
         <v>-0.12472</v>
@@ -4927,10 +4927,10 @@
     </row>
     <row r="287">
       <c r="A287" s="0">
-        <v>200.45772156084661</v>
+        <v>323.63549747033153</v>
       </c>
       <c r="B287" s="0">
-        <v>8.0890538033395174</v>
+        <v>1.6284760845383772</v>
       </c>
       <c r="C287" s="0">
         <v>-0.10287</v>
@@ -4944,10 +4944,10 @@
     </row>
     <row r="288">
       <c r="A288" s="0">
-        <v>201.15862268518524</v>
+        <v>324.76709011882917</v>
       </c>
       <c r="B288" s="0">
-        <v>8.0445269016697587</v>
+        <v>1.1479421579532811</v>
       </c>
       <c r="C288" s="0">
         <v>-0.048183999999999998</v>
@@ -4961,10 +4961,10 @@
     </row>
     <row r="289">
       <c r="A289" s="0">
-        <v>201.85952380952384</v>
+        <v>325.89868276732682</v>
       </c>
       <c r="B289" s="0">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C289" s="0">
         <v>-0.01308</v>
@@ -4973,7 +4973,7 @@
         <v>1440</v>
       </c>
       <c r="E289" s="0">
-        <v>0.009530814705262779</v>
+        <v>0.0071641429157009813</v>
       </c>
     </row>
     <row r="290">

</xml_diff>